<commit_message>
Update README, Add Files
</commit_message>
<xml_diff>
--- a/Modules/MiscFiles/MockOutput.xlsx
+++ b/Modules/MiscFiles/MockOutput.xlsx
@@ -457,11 +457,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>444185</v>
+        <v>495598</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,11 +477,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>116883</v>
+        <v>336813</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -497,11 +497,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>213456</v>
+        <v>263884</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,11 +517,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>254498</v>
+        <v>495424</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -537,7 +537,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>109571</v>
+        <v>437781</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -557,11 +557,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>410901</v>
+        <v>191387</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -577,11 +577,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>410872</v>
+        <v>243488</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -597,7 +597,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>231541</v>
+        <v>261361</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -617,11 +617,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>190123</v>
+        <v>143340</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -637,11 +637,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>266611</v>
+        <v>163298</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -657,7 +657,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>298222</v>
+        <v>432556</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -677,11 +677,11 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>395908</v>
+        <v>218390</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -697,7 +697,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>226813</v>
+        <v>177722</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>449551</v>
+        <v>420349</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -737,11 +737,11 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>203155</v>
+        <v>371566</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -757,11 +757,11 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>267041</v>
+        <v>471127</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -777,11 +777,11 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>185289</v>
+        <v>226075</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -797,7 +797,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>109569</v>
+        <v>150791</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -817,11 +817,11 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>163788</v>
+        <v>236422</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -837,11 +837,11 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>358554</v>
+        <v>261066</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -857,11 +857,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>463107</v>
+        <v>257024</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -877,7 +877,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>476617</v>
+        <v>434010</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -897,11 +897,11 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>180725</v>
+        <v>160615</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -917,7 +917,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>293008</v>
+        <v>287358</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>376398</v>
+        <v>385238</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -957,11 +957,11 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>474397</v>
+        <v>461694</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -977,11 +977,11 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>458643</v>
+        <v>448607</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -997,11 +997,11 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>135853</v>
+        <v>289240</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1017,11 +1017,11 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>132601</v>
+        <v>333336</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1037,7 +1037,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>262287</v>
+        <v>169688</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>371504</v>
+        <v>477474</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1077,11 +1077,11 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>169501</v>
+        <v>278870</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1097,11 +1097,11 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>360445</v>
+        <v>478694</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1117,11 +1117,11 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>468225</v>
+        <v>493863</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1137,11 +1137,11 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>123068</v>
+        <v>333526</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1157,11 +1157,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>127437</v>
+        <v>303795</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1177,11 +1177,11 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>211069</v>
+        <v>273497</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1197,11 +1197,11 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>488695</v>
+        <v>178218</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1217,11 +1217,11 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>492058</v>
+        <v>200586</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1237,7 +1237,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>449733</v>
+        <v>474124</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1257,11 +1257,11 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>449813</v>
+        <v>328894</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1277,11 +1277,11 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>395604</v>
+        <v>443011</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1297,11 +1297,11 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>276356</v>
+        <v>215601</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1317,11 +1317,11 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>217014</v>
+        <v>356736</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1337,7 +1337,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>451587</v>
+        <v>216818</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>254491</v>
+        <v>377768</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>232436</v>
+        <v>415977</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1397,11 +1397,11 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>412748</v>
+        <v>325056</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1417,11 +1417,11 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>285292</v>
+        <v>423196</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1437,11 +1437,11 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>181348</v>
+        <v>275684</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1457,11 +1457,11 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>331065</v>
+        <v>373998</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1477,11 +1477,11 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>431471</v>
+        <v>108935</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1497,11 +1497,11 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>385922</v>
+        <v>398717</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1517,11 +1517,11 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>375509</v>
+        <v>113685</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1537,11 +1537,11 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>254244</v>
+        <v>392982</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1557,11 +1557,11 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>421196</v>
+        <v>496948</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1577,11 +1577,11 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>225983</v>
+        <v>420868</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1597,11 +1597,11 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>491096</v>
+        <v>451908</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1617,11 +1617,11 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>271857</v>
+        <v>497494</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1637,11 +1637,11 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>174342</v>
+        <v>446572</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1657,7 +1657,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>128884</v>
+        <v>474539</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1677,11 +1677,11 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>277287</v>
+        <v>420890</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1697,11 +1697,11 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>467321</v>
+        <v>431636</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1717,11 +1717,11 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>465635</v>
+        <v>250109</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1737,7 +1737,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>233594</v>
+        <v>219275</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -1757,11 +1757,11 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>438404</v>
+        <v>344879</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1777,7 +1777,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>472232</v>
+        <v>358171</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>140080</v>
+        <v>335642</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -1817,11 +1817,11 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>280990</v>
+        <v>247969</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1837,11 +1837,11 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>235976</v>
+        <v>473370</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1857,11 +1857,11 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>407959</v>
+        <v>107787</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1877,11 +1877,11 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>407602</v>
+        <v>228741</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1897,11 +1897,11 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>401955</v>
+        <v>494371</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1917,7 +1917,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>401313</v>
+        <v>308428</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -1937,11 +1937,11 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>239922</v>
+        <v>312091</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1957,7 +1957,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>133708</v>
+        <v>329278</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>145990</v>
+        <v>280363</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -1997,11 +1997,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>278865</v>
+        <v>106422</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2017,11 +2017,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>251210</v>
+        <v>479694</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2037,11 +2037,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>474175</v>
+        <v>165416</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2057,7 +2057,7 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>316932</v>
+        <v>422621</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2077,11 +2077,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>248767</v>
+        <v>315531</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2097,11 +2097,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>303407</v>
+        <v>224936</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2117,11 +2117,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>164574</v>
+        <v>286719</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2137,7 +2137,7 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>416123</v>
+        <v>203021</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -2157,11 +2157,11 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>498904</v>
+        <v>278609</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2177,7 +2177,7 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>289943</v>
+        <v>185251</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -2197,11 +2197,11 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>278282</v>
+        <v>399616</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2217,11 +2217,11 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>437040</v>
+        <v>134340</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2237,11 +2237,11 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>278445</v>
+        <v>385080</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2257,11 +2257,11 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>332772</v>
+        <v>232316</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2277,11 +2277,11 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>114458</v>
+        <v>392256</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2297,7 +2297,7 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>488039</v>
+        <v>448186</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>435668</v>
+        <v>328248</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -2337,11 +2337,11 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>204857</v>
+        <v>282688</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2357,11 +2357,11 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>453973</v>
+        <v>399661</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2377,7 +2377,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>368597</v>
+        <v>388296</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -2397,11 +2397,11 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>329011</v>
+        <v>374858</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2417,11 +2417,11 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>416338</v>
+        <v>260934</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2437,11 +2437,11 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>226072</v>
+        <v>329263</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2457,11 +2457,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>384555</v>
+        <v>334594</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2477,11 +2477,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>410482</v>
+        <v>348325</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2497,11 +2497,11 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>338565</v>
+        <v>171443</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2517,11 +2517,11 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>341223</v>
+        <v>310117</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2537,11 +2537,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>302778</v>
+        <v>244022</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2557,11 +2557,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>439337</v>
+        <v>166604</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2577,7 +2577,7 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>316038</v>
+        <v>439960</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -2597,11 +2597,11 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>104597</v>
+        <v>434419</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2617,7 +2617,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>183689</v>
+        <v>307165</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -2637,11 +2637,11 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>254290</v>
+        <v>310477</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2657,7 +2657,7 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>267746</v>
+        <v>139836</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -2677,11 +2677,11 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>147977</v>
+        <v>352402</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2697,11 +2697,11 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>430906</v>
+        <v>344749</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2717,7 +2717,7 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>152466</v>
+        <v>422707</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -2737,11 +2737,11 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>405464</v>
+        <v>139983</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2757,7 +2757,7 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>214583</v>
+        <v>100816</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -2777,11 +2777,11 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>282852</v>
+        <v>456745</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2797,7 +2797,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>145348</v>
+        <v>394250</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -2817,11 +2817,11 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>341948</v>
+        <v>306586</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2837,11 +2837,11 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>206636</v>
+        <v>164298</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2857,11 +2857,11 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>371388</v>
+        <v>333779</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2877,11 +2877,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>374831</v>
+        <v>293003</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2897,11 +2897,11 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>427035</v>
+        <v>264007</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2917,11 +2917,11 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>418654</v>
+        <v>420967</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2937,7 +2937,7 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>224432</v>
+        <v>386179</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -2957,11 +2957,11 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>249277</v>
+        <v>276327</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2977,11 +2977,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>187430</v>
+        <v>183492</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2997,7 +2997,7 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>119457</v>
+        <v>155770</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -3017,11 +3017,11 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>218095</v>
+        <v>224706</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3037,11 +3037,11 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>296919</v>
+        <v>392912</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3057,11 +3057,11 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>365505</v>
+        <v>225036</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3077,11 +3077,11 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>372980</v>
+        <v>354675</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3097,11 +3097,11 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>263960</v>
+        <v>166999</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3117,11 +3117,11 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>224295</v>
+        <v>343682</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3137,11 +3137,11 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>279483</v>
+        <v>386182</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3157,11 +3157,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>267952</v>
+        <v>419052</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3177,11 +3177,11 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>446953</v>
+        <v>146949</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3197,11 +3197,11 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>315438</v>
+        <v>390879</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3217,11 +3217,11 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>373216</v>
+        <v>429739</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3237,11 +3237,11 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>464074</v>
+        <v>360813</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3257,7 +3257,7 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>235876</v>
+        <v>407737</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -3277,11 +3277,11 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>442435</v>
+        <v>366853</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3297,11 +3297,11 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>283597</v>
+        <v>455336</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -3317,11 +3317,11 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>258823</v>
+        <v>111812</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -3337,11 +3337,11 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>475269</v>
+        <v>410546</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3357,11 +3357,11 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>348235</v>
+        <v>354581</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3377,11 +3377,11 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>213846</v>
+        <v>292916</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3397,11 +3397,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>272749</v>
+        <v>368557</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -3417,7 +3417,7 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>479919</v>
+        <v>416576</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -3437,11 +3437,11 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>277524</v>
+        <v>388915</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3457,11 +3457,11 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>250575</v>
+        <v>423788</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3477,11 +3477,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>426008</v>
+        <v>289479</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3497,11 +3497,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>323314</v>
+        <v>350679</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3517,11 +3517,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>314401</v>
+        <v>375336</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3537,7 +3537,7 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>473945</v>
+        <v>311751</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -3557,11 +3557,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>300376</v>
+        <v>150851</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3577,11 +3577,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>139460</v>
+        <v>337519</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3597,11 +3597,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>228832</v>
+        <v>353687</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3617,11 +3617,11 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>246758</v>
+        <v>318015</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3637,7 +3637,7 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>461268</v>
+        <v>430509</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -3657,7 +3657,7 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>308072</v>
+        <v>263712</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -3677,11 +3677,11 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>451554</v>
+        <v>346325</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3697,11 +3697,11 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>170827</v>
+        <v>398094</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3717,11 +3717,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>343218</v>
+        <v>335582</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3737,11 +3737,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>433119</v>
+        <v>399327</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3757,11 +3757,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>345952</v>
+        <v>271616</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3777,7 +3777,7 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>238423</v>
+        <v>401869</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -3797,11 +3797,11 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>202407</v>
+        <v>261213</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3817,11 +3817,11 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>437345</v>
+        <v>423914</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3837,11 +3837,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>150572</v>
+        <v>180689</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3857,7 +3857,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>108623</v>
+        <v>124107</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -3877,7 +3877,7 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>332459</v>
+        <v>161594</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -3897,11 +3897,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>109722</v>
+        <v>194882</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3917,11 +3917,11 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>460093</v>
+        <v>403958</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3937,11 +3937,11 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>154641</v>
+        <v>100570</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>HOST</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3957,11 +3957,11 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>339339</v>
+        <v>379674</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3977,7 +3977,7 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>103872</v>
+        <v>361677</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -3997,11 +3997,11 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>143834</v>
+        <v>184178</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -4017,11 +4017,11 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>136525</v>
+        <v>212317</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -4037,7 +4037,7 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>303130</v>
+        <v>491168</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>252153</v>
+        <v>369316</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -4077,7 +4077,7 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>228836</v>
+        <v>403483</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -4097,11 +4097,11 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>334710</v>
+        <v>241414</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -4117,11 +4117,11 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>104753</v>
+        <v>285984</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -4137,11 +4137,11 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>333456</v>
+        <v>309558</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -4157,11 +4157,11 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>292393</v>
+        <v>219853</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HESTA</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -4177,11 +4177,11 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>346365</v>
+        <v>179486</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -4197,11 +4197,11 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>410344</v>
+        <v>192063</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -4217,7 +4217,7 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>177446</v>
+        <v>296531</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>294497</v>
+        <v>455272</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
@@ -4257,11 +4257,11 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>165242</v>
+        <v>483428</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -4277,11 +4277,11 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>337992</v>
+        <v>230875</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -4297,11 +4297,11 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>466123</v>
+        <v>380513</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -4317,7 +4317,7 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>162336</v>
+        <v>201696</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
@@ -4337,11 +4337,11 @@
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>310745</v>
+        <v>395186</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -4357,11 +4357,11 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>210746</v>
+        <v>215274</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>CBUS</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -4377,7 +4377,7 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>223922</v>
+        <v>345259</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
@@ -4397,11 +4397,11 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>147537</v>
+        <v>366113</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>CBUS</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -4417,11 +4417,11 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>265302</v>
+        <v>395326</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>HESTA</t>
+          <t>AS</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -4437,11 +4437,11 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>408684</v>
+        <v>187687</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>HOST</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">

</xml_diff>